<commit_message>
updated sprint backlog and backlog
</commit_message>
<xml_diff>
--- a/docs/backlog.xlsx
+++ b/docs/backlog.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="68">
   <si>
     <t>Project Name</t>
   </si>
@@ -50,9 +50,18 @@
     <t>Estimation</t>
   </si>
   <si>
+    <t>Как незарегистрированный пользователь я хочу зарегистрироваться в системе, чтобы использовать ее функции в полном объеме</t>
+  </si>
+  <si>
     <t>Открыть приложение, нажать на кнопку "Зарегистрироваться", ввести данные для регистрации</t>
   </si>
   <si>
+    <t>Как зарегистрированный пользователь, я хочу войти в систему, чтобы использовать ее функции в полном объеме</t>
+  </si>
+  <si>
+    <t>Нажать на кнопку "Войти", ввести логин и пароль</t>
+  </si>
+  <si>
     <t>Как незарегистрированный пользователь, я хочу просмотреть карты других пользователей, чтобы узнать, где находится интересующий меня объект</t>
   </si>
   <si>
@@ -71,6 +80,9 @@
     <t>Войти в систему, выбрать карту, создать метку, ввести о ней необходимую информацию в текстовые поля</t>
   </si>
   <si>
+    <t>Как пользователь, я хочу осуществлять поиск меток по определенным характеристикам, чтобы быстро находить интересующие меня объекты</t>
+  </si>
+  <si>
     <t>Открыть приложение, выбрать интересующую карту, нажать кнопку "Поиск", выбрать параметры поиска</t>
   </si>
   <si>
@@ -80,6 +92,9 @@
     <t>Открыть приложение, выбрать интересующую карту, нажать кнопку "Сортировка", выбрать параметры сортировки</t>
   </si>
   <si>
+    <t>Как зарегистрированный пользователь, я хочу добавлять метки на карты других пользователей, чтобы они становились полезнее</t>
+  </si>
+  <si>
     <t>Войти в систему, найти интересующую карту, нажав "Поиск карты", добавить на нее метку</t>
   </si>
   <si>
@@ -161,9 +176,6 @@
     <t>Шилин</t>
   </si>
   <si>
-    <t>oleksandr.shylin@nure.ua</t>
-  </si>
-  <si>
     <t>Ирина</t>
   </si>
   <si>
@@ -182,9 +194,6 @@
     <t>Рассоха</t>
   </si>
   <si>
-    <t>бизнес-аналитик</t>
-  </si>
-  <si>
     <t>olha.rassokha@nure.ua</t>
   </si>
   <si>
@@ -194,9 +203,6 @@
     <t>Никонова</t>
   </si>
   <si>
-    <t>дизайнер</t>
-  </si>
-  <si>
     <t>anna.nikonova@nure.ua</t>
   </si>
   <si>
@@ -206,19 +212,19 @@
     <t>Камянский</t>
   </si>
   <si>
-    <t>ihor.kamianskiy@nure.ua</t>
-  </si>
-  <si>
     <t>srs</t>
   </si>
   <si>
-    <t>Как незарегистрированный пользователь я хочу зарегистрироваться в системе, чтобы иметь доступ к редактированию карт</t>
-  </si>
-  <si>
-    <t>Как пользователь, я хочу осуществлять поиск меток по определенным характеристикам, чтобы быстро находить интересующие меня объекты среди множества остальных</t>
-  </si>
-  <si>
-    <t>Как зарегистрированный пользователь, я хочу добавлять метки на карты других пользователей, чтобы наполнять их</t>
+    <t>oleksandr.shylin1@nure.ua</t>
+  </si>
+  <si>
+    <t>тестировщик, дизайнер</t>
+  </si>
+  <si>
+    <t>kamyanskiy.i@gmail.com</t>
+  </si>
+  <si>
+    <t>бизнес-аналитик, проектировщик базы данных</t>
   </si>
 </sst>
 </file>
@@ -313,7 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -338,6 +344,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -708,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G42"/>
+  <dimension ref="A2:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,10 +774,10 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G5" s="4">
         <v>5</v>
@@ -784,75 +791,75 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>3</v>
       </c>
-      <c r="B7" s="4">
-        <v>100</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G7" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>4</v>
       </c>
       <c r="B8" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G8" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>5</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="B9" s="4">
+        <v>90</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="G9" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>6</v>
       </c>
@@ -860,53 +867,53 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="G10" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>7</v>
       </c>
-      <c r="B11" s="4">
-        <v>80</v>
-      </c>
-      <c r="C11" s="4">
-        <v>1</v>
-      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
       <c r="E11" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="G11" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>8</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="B12" s="4">
+        <v>80</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
       <c r="E12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="G12" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>9</v>
       </c>
@@ -914,16 +921,16 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G13" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>10</v>
       </c>
@@ -931,55 +938,63 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G14" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>11</v>
       </c>
-      <c r="B15" s="4">
-        <v>70</v>
-      </c>
-      <c r="C15" s="4">
-        <v>1</v>
-      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G15" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>12</v>
+      </c>
+      <c r="B16" s="4">
+        <v>70</v>
+      </c>
       <c r="C16" s="4">
         <v>1</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="E16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
       <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
@@ -1073,48 +1088,39 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F31" s="10" t="s">
+      <c r="B31" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="12" t="s">
+      <c r="A32" s="9"/>
+      <c r="B32" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F32" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1145,31 +1151,31 @@
         <v>45</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>41</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F35" s="13" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1181,10 +1187,10 @@
         <v>52</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="F36" s="13" t="s">
         <v>54</v>
@@ -1199,40 +1205,50 @@
         <v>56</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E37" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F37" s="13" t="s">
         <v>57</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="D38" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F38" s="14" t="s">
         <v>60</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F38" s="13" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
+      <c r="B39" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
@@ -1258,15 +1274,23 @@
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
     </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F32" r:id="rId1"/>
-    <hyperlink ref="F33" r:id="rId2"/>
-    <hyperlink ref="F34" r:id="rId3"/>
-    <hyperlink ref="F35" r:id="rId4"/>
-    <hyperlink ref="F36" r:id="rId5"/>
-    <hyperlink ref="F37" r:id="rId6"/>
-    <hyperlink ref="F38" r:id="rId7"/>
+    <hyperlink ref="F33" r:id="rId1"/>
+    <hyperlink ref="F34" r:id="rId2"/>
+    <hyperlink ref="F35" r:id="rId3"/>
+    <hyperlink ref="F36" r:id="rId4"/>
+    <hyperlink ref="F37" r:id="rId5"/>
+    <hyperlink ref="F38" r:id="rId6"/>
+    <hyperlink ref="F39" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>